<commit_message>
[fixed] added sp chosen instead of sp_current in dofile
</commit_message>
<xml_diff>
--- a/Project-v1/Documents/Memory/NO_haza_no_forw_SOLUTION/no_haza_no_forw_SOLUTION_MEM.xlsx
+++ b/Project-v1/Documents/Memory/NO_haza_no_forw_SOLUTION/no_haza_no_forw_SOLUTION_MEM.xlsx
@@ -132,9 +132,6 @@
     <t>M[200] = R2 =F5</t>
   </si>
   <si>
-    <t>R3 = M[202] = F5</t>
-  </si>
-  <si>
     <t>R4 = M[200] = F5</t>
   </si>
   <si>
@@ -145,6 +142,9 @@
   </si>
   <si>
     <t>M[202] = R1 = 0CDAFE19</t>
+  </si>
+  <si>
+    <t>R3 = M[202] = 0CDAFE19</t>
   </si>
 </sst>
 </file>
@@ -216,7 +216,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -237,31 +237,32 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -566,7 +567,7 @@
   <dimension ref="A1:AW37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AM23" sqref="AM23"/>
+      <selection activeCell="AJ34" sqref="AJ34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -576,26 +577,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14" t="s">
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
     </row>
     <row r="2" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
       <c r="G2" t="s">
         <v>1</v>
       </c>
@@ -611,25 +612,25 @@
       <c r="K2" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="17" t="s">
+      <c r="O2" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="P2" s="17"/>
-      <c r="Q2" s="17"/>
-      <c r="R2" s="17"/>
-      <c r="S2" s="17"/>
-      <c r="T2" s="17"/>
-      <c r="U2" s="17"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="15"/>
+      <c r="S2" s="15"/>
+      <c r="T2" s="15"/>
+      <c r="U2" s="15"/>
     </row>
     <row r="3" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
       <c r="H3" t="s">
         <v>1</v>
       </c>
@@ -645,20 +646,20 @@
       <c r="L3" t="s">
         <v>5</v>
       </c>
-      <c r="Q3" s="17" t="s">
+      <c r="Q3" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="R3" s="17"/>
-      <c r="S3" s="17"/>
-      <c r="T3" s="17"/>
-      <c r="U3" s="17"/>
+      <c r="R3" s="15"/>
+      <c r="S3" s="15"/>
+      <c r="T3" s="15"/>
+      <c r="U3" s="15"/>
     </row>
     <row r="4" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
       <c r="I4" t="s">
         <v>1</v>
       </c>
@@ -674,19 +675,19 @@
       <c r="M4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="S4" s="17" t="s">
+      <c r="S4" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="T4" s="17"/>
-      <c r="U4" s="17"/>
-      <c r="V4" s="17"/>
+      <c r="T4" s="15"/>
+      <c r="U4" s="15"/>
+      <c r="V4" s="15"/>
     </row>
     <row r="5" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
       <c r="J5" s="4" t="s">
         <v>1</v>
       </c>
@@ -710,12 +711,12 @@
       <c r="R5" s="4"/>
       <c r="S5" s="4"/>
       <c r="T5" s="6"/>
-      <c r="U5" s="17" t="s">
+      <c r="U5" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="V5" s="17"/>
-      <c r="W5" s="17"/>
-      <c r="X5" s="17"/>
+      <c r="V5" s="15"/>
+      <c r="W5" s="15"/>
+      <c r="X5" s="15"/>
       <c r="Y5" s="4"/>
       <c r="Z5" s="4"/>
       <c r="AA5" s="4"/>
@@ -737,11 +738,11 @@
       <c r="AQ5" s="4"/>
     </row>
     <row r="6" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="D6" s="21" t="s">
+      <c r="D6" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4" t="s">
         <v>1</v>
@@ -790,11 +791,11 @@
       <c r="AQ6" s="4"/>
     </row>
     <row r="7" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="D7" s="21" t="s">
+      <c r="D7" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
       <c r="L7" s="4" t="s">
@@ -843,11 +844,11 @@
       <c r="AQ7" s="4"/>
     </row>
     <row r="8" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
       <c r="D8" s="20" t="s">
         <v>17</v>
       </c>
@@ -885,19 +886,19 @@
       <c r="AH8" s="4"/>
       <c r="AI8" s="4"/>
       <c r="AJ8" s="4"/>
-      <c r="AT8" s="17" t="s">
+      <c r="AT8" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="AU8" s="17"/>
-      <c r="AV8" s="17"/>
-      <c r="AW8" s="17"/>
+      <c r="AU8" s="15"/>
+      <c r="AV8" s="15"/>
+      <c r="AW8" s="15"/>
     </row>
     <row r="9" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
       <c r="D9" s="18" t="s">
         <v>16</v>
       </c>
@@ -941,22 +942,22 @@
       <c r="AG9" s="6"/>
       <c r="AH9" s="6"/>
       <c r="AI9" s="6"/>
-      <c r="AT9" s="17" t="s">
+      <c r="AT9" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="AU9" s="17"/>
-      <c r="AV9" s="17"/>
-      <c r="AW9" s="17"/>
+      <c r="AU9" s="15"/>
+      <c r="AV9" s="15"/>
+      <c r="AW9" s="15"/>
     </row>
     <row r="10" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
-      <c r="D10" s="19" t="s">
+      <c r="D10" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
@@ -983,33 +984,33 @@
       <c r="W10" s="4"/>
       <c r="X10" s="4"/>
       <c r="Y10" s="4"/>
-      <c r="Z10" s="17" t="s">
+      <c r="Z10" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="AA10" s="17"/>
-      <c r="AB10" s="17"/>
-      <c r="AC10" s="17"/>
-      <c r="AD10" s="17"/>
-      <c r="AE10" s="17"/>
-      <c r="AF10" s="17"/>
-      <c r="AG10" s="17"/>
-      <c r="AH10" s="17"/>
-      <c r="AI10" s="17"/>
-      <c r="AJ10" s="17"/>
+      <c r="AA10" s="15"/>
+      <c r="AB10" s="15"/>
+      <c r="AC10" s="15"/>
+      <c r="AD10" s="15"/>
+      <c r="AE10" s="15"/>
+      <c r="AF10" s="15"/>
+      <c r="AG10" s="15"/>
+      <c r="AH10" s="15"/>
+      <c r="AI10" s="15"/>
+      <c r="AJ10" s="15"/>
       <c r="AO10" s="4"/>
       <c r="AP10" s="4"/>
       <c r="AQ10" s="4"/>
-      <c r="AT10" s="17" t="s">
+      <c r="AT10" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="AU10" s="17"/>
-      <c r="AV10" s="17"/>
-      <c r="AW10" s="17"/>
+      <c r="AU10" s="15"/>
+      <c r="AV10" s="15"/>
+      <c r="AW10" s="15"/>
     </row>
     <row r="11" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
+      <c r="A11" s="17"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
       <c r="D11" s="18" t="s">
         <v>22</v>
       </c>
@@ -1042,15 +1043,15 @@
       <c r="X11" s="4"/>
       <c r="Y11" s="4"/>
       <c r="Z11" s="4"/>
-      <c r="AB11" s="17" t="s">
+      <c r="AB11" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="AC11" s="17"/>
-      <c r="AD11" s="17"/>
-      <c r="AE11" s="17"/>
-      <c r="AF11" s="17"/>
-      <c r="AG11" s="17"/>
-      <c r="AH11" s="17"/>
+      <c r="AC11" s="15"/>
+      <c r="AD11" s="15"/>
+      <c r="AE11" s="15"/>
+      <c r="AF11" s="15"/>
+      <c r="AG11" s="15"/>
+      <c r="AH11" s="15"/>
       <c r="AI11" s="6"/>
       <c r="AJ11" s="6"/>
       <c r="AK11" s="6"/>
@@ -1060,22 +1061,22 @@
       <c r="AO11" s="4"/>
       <c r="AP11" s="4"/>
       <c r="AQ11" s="4"/>
-      <c r="AT11" s="17" t="s">
+      <c r="AT11" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="AU11" s="17"/>
-      <c r="AV11" s="17"/>
-      <c r="AW11" s="17"/>
+      <c r="AU11" s="15"/>
+      <c r="AV11" s="15"/>
+      <c r="AW11" s="15"/>
     </row>
     <row r="12" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
-      <c r="D12" s="15" t="s">
+      <c r="D12" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
@@ -1128,11 +1129,11 @@
       <c r="A13" s="9"/>
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
-      <c r="D13" s="15" t="s">
+      <c r="D13" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
@@ -1182,11 +1183,11 @@
       <c r="AW13" s="10"/>
     </row>
     <row r="14" spans="1:49" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
       <c r="D14" s="20" t="s">
         <v>24</v>
       </c>
@@ -1235,11 +1236,11 @@
       <c r="AQ14" s="4"/>
     </row>
     <row r="15" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
+      <c r="A15" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
       <c r="D15" s="18" t="s">
         <v>25</v>
       </c>
@@ -1277,15 +1278,15 @@
       </c>
       <c r="AB15" s="4"/>
       <c r="AC15" s="4"/>
-      <c r="AJ15" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="AK15" s="22"/>
-      <c r="AL15" s="22"/>
-      <c r="AM15" s="22"/>
-      <c r="AN15" s="22"/>
-      <c r="AO15" s="22"/>
-      <c r="AP15" s="22"/>
+      <c r="AJ15" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="AK15" s="14"/>
+      <c r="AL15" s="14"/>
+      <c r="AM15" s="14"/>
+      <c r="AN15" s="14"/>
+      <c r="AO15" s="14"/>
+      <c r="AP15" s="14"/>
       <c r="AQ15" s="8"/>
       <c r="AR15" s="8"/>
       <c r="AS15" s="8"/>
@@ -1336,16 +1337,19 @@
       <c r="AD16" s="4"/>
       <c r="AE16" s="4"/>
       <c r="AF16" s="4"/>
-      <c r="AK16" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="AL16" s="17"/>
-      <c r="AM16" s="17"/>
-      <c r="AN16" s="17"/>
-      <c r="AO16" s="17"/>
-      <c r="AP16" s="17"/>
-      <c r="AQ16" s="17"/>
-      <c r="AR16" s="6"/>
+      <c r="AK16" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="AL16" s="23"/>
+      <c r="AM16" s="23"/>
+      <c r="AN16" s="23"/>
+      <c r="AO16" s="23"/>
+      <c r="AP16" s="23"/>
+      <c r="AQ16" s="23"/>
+      <c r="AR16" s="23"/>
+      <c r="AS16" s="5"/>
+      <c r="AT16" s="5"/>
+      <c r="AU16" s="5"/>
     </row>
     <row r="17" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
@@ -1394,21 +1398,21 @@
       <c r="AE17" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="AM17" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="AN17" s="17"/>
-      <c r="AO17" s="17"/>
-      <c r="AP17" s="17"/>
-      <c r="AQ17" s="17"/>
-      <c r="AR17" s="17"/>
-      <c r="AS17" s="17"/>
+      <c r="AM17" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="AN17" s="15"/>
+      <c r="AO17" s="15"/>
+      <c r="AP17" s="15"/>
+      <c r="AQ17" s="15"/>
+      <c r="AR17" s="15"/>
+      <c r="AS17" s="15"/>
       <c r="AT17" s="6"/>
     </row>
     <row r="18" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A18" s="14"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
+      <c r="A18" s="17"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
       <c r="D18" s="18"/>
       <c r="E18" s="18"/>
       <c r="F18" s="18"/>
@@ -1449,69 +1453,57 @@
     </row>
     <row r="33" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C33" s="2"/>
-      <c r="D33" s="14" t="s">
+      <c r="D33" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="E33" s="14"/>
-      <c r="F33" s="14"/>
+      <c r="E33" s="17"/>
+      <c r="F33" s="17"/>
     </row>
     <row r="34" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C34" s="3"/>
-      <c r="D34" s="14" t="s">
+      <c r="D34" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="E34" s="14"/>
-      <c r="F34" s="14"/>
+      <c r="E34" s="17"/>
+      <c r="F34" s="17"/>
     </row>
     <row r="35" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C35" s="5"/>
-      <c r="D35" s="14" t="s">
+      <c r="D35" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E35" s="14"/>
-      <c r="F35" s="14"/>
+      <c r="E35" s="17"/>
+      <c r="F35" s="17"/>
     </row>
     <row r="36" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C36" s="8"/>
-      <c r="D36" s="14" t="s">
+      <c r="D36" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="E36" s="14"/>
-      <c r="F36" s="14"/>
+      <c r="E36" s="17"/>
+      <c r="F36" s="17"/>
     </row>
     <row r="37" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C37" s="12"/>
-      <c r="D37" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="E37" s="14"/>
-      <c r="F37" s="14"/>
+      <c r="D37" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="E37" s="17"/>
+      <c r="F37" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="45">
-    <mergeCell ref="AB11:AH11"/>
-    <mergeCell ref="AT10:AW10"/>
-    <mergeCell ref="AT11:AW11"/>
-    <mergeCell ref="Z10:AJ10"/>
-    <mergeCell ref="AT8:AW8"/>
-    <mergeCell ref="X9:AF9"/>
-    <mergeCell ref="AT9:AW9"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="S4:V4"/>
-    <mergeCell ref="O2:U2"/>
-    <mergeCell ref="Q3:U3"/>
-    <mergeCell ref="U5:X5"/>
-    <mergeCell ref="W8:AA8"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="D5:F5"/>
+  <mergeCells count="44">
+    <mergeCell ref="D37:F37"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="AI14:AO14"/>
+    <mergeCell ref="AM17:AS17"/>
+    <mergeCell ref="D36:F36"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="D35:F35"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="D18:F18"/>
     <mergeCell ref="A18:C18"/>
     <mergeCell ref="D15:F15"/>
     <mergeCell ref="A15:C15"/>
@@ -1522,18 +1514,29 @@
     <mergeCell ref="A11:C11"/>
     <mergeCell ref="D14:F14"/>
     <mergeCell ref="A14:C14"/>
-    <mergeCell ref="D37:F37"/>
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="AI14:AO14"/>
-    <mergeCell ref="AK16:AQ16"/>
-    <mergeCell ref="AM17:AS17"/>
-    <mergeCell ref="D36:F36"/>
-    <mergeCell ref="D33:F33"/>
-    <mergeCell ref="D34:F34"/>
-    <mergeCell ref="D35:F35"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="U5:X5"/>
+    <mergeCell ref="W8:AA8"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="S4:V4"/>
+    <mergeCell ref="O2:U2"/>
+    <mergeCell ref="Q3:U3"/>
+    <mergeCell ref="AB11:AH11"/>
+    <mergeCell ref="AT10:AW10"/>
+    <mergeCell ref="AT11:AW11"/>
+    <mergeCell ref="Z10:AJ10"/>
+    <mergeCell ref="AT8:AW8"/>
+    <mergeCell ref="X9:AF9"/>
+    <mergeCell ref="AT9:AW9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>